<commit_message>
Agregar solucionario del trabajo 1
</commit_message>
<xml_diff>
--- a/Trabajo 1/Solucionario/Tablas_de_verdad.xlsx
+++ b/Trabajo 1/Solucionario/Tablas_de_verdad.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erika\OneDrive\Desktop\Clases-Eafit\Introduccion-a-la-programacion\Trabajo 1\Solucionario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5606297E-8A4F-443E-8222-B219FE39D265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EE0A42-42C9-4038-A88F-FF19838C289B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C6EB9CA2-1308-48BC-8CAE-28EFB6AE9909}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{C6EB9CA2-1308-48BC-8CAE-28EFB6AE9909}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla 1" sheetId="1" r:id="rId1"/>
@@ -500,7 +500,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -637,7 +637,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -754,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BCCAA8-6995-461D-B299-DE534CDFE787}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{807BCFEC-4DC1-4941-B469-F639D08C9854}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>

</xml_diff>